<commit_message>
updated filekey to switch 50 and 103
</commit_message>
<xml_diff>
--- a/phage_AGK_25_filekey.xlsx
+++ b/phage_AGK_25_filekey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asim.khan\Desktop\Miseq_Runs\ncRNA_Project\Phage_Analysis\Multiplexed_Phage_Recombitrons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2102BEF4-D8AE-40D2-BF3E-511ACC1D99E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A61DBE1-BE6A-4A3C-8D3E-9C86540AA4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="17460" windowHeight="10380" xr2:uid="{5092B66F-C68F-3B49-A10E-6D9E2CEABAC1}"/>
   </bookViews>
@@ -646,7 +646,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
@@ -724,10 +724,10 @@
         <v>41</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="6">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>6</v>
@@ -736,10 +736,10 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>9</v>
@@ -753,10 +753,10 @@
         <v>42</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" s="6">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>6</v>
@@ -765,10 +765,10 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>9</v>
@@ -1225,12 +1225,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.8">
       <c r="A21" s="5"/>
-      <c r="B21" s="4"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="4"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>

</xml_diff>